<commit_message>
flujo carga de datos
</commit_message>
<xml_diff>
--- a/core/static/core/LayOut.xlsx
+++ b/core/static/core/LayOut.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3929B7E-F7DB-4787-89E7-B5B53C975943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataTracing\prototipo noe\dtpython1\core\static\core\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCD7CE8-3DBF-4DEE-ACED-1EEB8B470CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{66819AA7-9B69-4E02-892B-1F8F1D2B1481}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT INPUTS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -19,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,34 +34,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>CUENTA ENCRIPTADA</t>
-  </si>
-  <si>
-    <t>PRODUCTO</t>
-  </si>
-  <si>
-    <t>CODIGO DEL PAIS</t>
-  </si>
-  <si>
-    <t>FECHA DE LA REVISION</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>NOMBRE DEL CLIENTE</t>
+  </si>
+  <si>
+    <t>SUBPRODUCTO</t>
+  </si>
+  <si>
+    <t>Fecha de la revisión</t>
+  </si>
+  <si>
+    <t>Nombre de los atributos</t>
+  </si>
+  <si>
+    <t>Codigo del país</t>
   </si>
   <si>
     <t>FEED ID</t>
   </si>
   <si>
-    <t>NOMBRE D ELOS ATRIBUTOS</t>
-  </si>
-  <si>
-    <t>VALOR</t>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t># PRODUCTO</t>
+  </si>
+  <si>
+    <t>INSTRUMENTO</t>
+  </si>
+  <si>
+    <t>DESENCRIPTADO ( # De Cuenta)</t>
+  </si>
+  <si>
+    <t>(PRODUCTO)
+Descripción</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # CLIENTE</t>
+  </si>
+  <si>
+    <t>Cuenta Encriptada</t>
+  </si>
+  <si>
+    <t>STATUS DE LA CTA  
+(liquidado, castigado, activo, etc)</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,8 +95,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +127,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,15 +155,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -110,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -405,48 +513,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11035A7E-8E95-4316-BB11-9C9AF52D60DD}">
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="21.21875" style="4"/>
+    <col min="5" max="5" width="56.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" style="4"/>
+    <col min="7" max="7" width="25.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="21.21875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="O1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="17"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="17"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="17"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="17"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="17"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="17"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="17"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>